<commit_message>
update isFormEditable field in update form method
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.No.</t>
   </si>
@@ -23,52 +23,28 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>what is ur namee ?</t>
+    <t>Star Based</t>
   </si>
   <si>
-    <t>ashikkk Siddiq M</t>
+    <t>4.5</t>
   </si>
   <si>
-    <t>What u will prefer Work from home/office ?</t>
+    <t>Descriptive</t>
   </si>
   <si>
-    <t>office</t>
+    <t>dfadfasf</t>
   </si>
   <si>
-    <t>what is ur name ?</t>
+    <t>Single choice</t>
   </si>
   <si>
-    <t>Syed Ashik Siddiq M</t>
+    <t>Option 1</t>
   </si>
   <si>
-    <t>Rate AU Program out of 5 ?</t>
+    <t>Multiple Choice</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>what is ur mame ?</t>
-  </si>
-  <si>
-    <t>Ashik Siddiq M</t>
-  </si>
-  <si>
-    <t>What is ur hobby?</t>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>what is your name ?</t>
-  </si>
-  <si>
-    <t>Syed Siddiq M</t>
-  </si>
-  <si>
-    <t>what is ur names ?</t>
-  </si>
-  <si>
-    <t>Siddiq M</t>
+    <t>Option 1,Option 2</t>
   </si>
 </sst>
 </file>
@@ -128,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -138,8 +114,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="6.4375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="40.52734375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="18.94921875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.09375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="17.15234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -197,50 +173,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>